<commit_message>
Versión lista a revisión
</commit_message>
<xml_diff>
--- a/datos/datos_fecha_fija.xlsx
+++ b/datos/datos_fecha_fija.xlsx
@@ -50,11 +50,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -70,6 +71,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -114,13 +122,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -140,10 +152,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -209,6 +221,7 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">

</xml_diff>

<commit_message>
Datos para ejecutar el robot en el curso de prueba
</commit_message>
<xml_diff>
--- a/datos/datos_fecha_fija.xlsx
+++ b/datos/datos_fecha_fija.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">CURSOS_ID</t>
   </si>
@@ -37,10 +37,19 @@
     <t xml:space="preserve">CPS1.1</t>
   </si>
   <si>
-    <t xml:space="preserve">15-09-2018-00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16-09-2018-00:00</t>
+    <t xml:space="preserve">15-09-2018-6:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-09-2018-9:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CPS1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15-09-2018-12:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16-09-2018-15:00</t>
   </si>
 </sst>
 </file>
@@ -50,7 +59,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -71,6 +80,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -122,7 +144,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -131,7 +153,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,7 +185,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -180,11 +210,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>5805</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>13317</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -194,90 +224,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>5804</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>13317</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>5803</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>5802</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>5801</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
-        <v>5800</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
-        <v>5799</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>